<commit_message>
Minor clean up to the radar spreadsheet.
</commit_message>
<xml_diff>
--- a/radars.xlsx
+++ b/radars.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/767eab0b527c63f4/Documents/Engineering/Radar Cross Section/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tj\Documents\Engineering\Radar Cross Section\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="234" documentId="8_{55B03561-656D-4867-8E19-D71C9E2769CF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{03DBE32E-BA72-41C3-B935-A34674A88464}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCD57370-8CBC-4FFA-9B3E-049DA1CADADA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17460" yWindow="5880" windowWidth="17616" windowHeight="17532" xr2:uid="{4644795B-AF5F-4458-9974-60729102D395}"/>
+    <workbookView xWindow="15870" yWindow="9840" windowWidth="27060" windowHeight="15600" xr2:uid="{4644795B-AF5F-4458-9974-60729102D395}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="55">
   <si>
     <t>Name</t>
   </si>
@@ -561,23 +561,23 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E14" sqref="E14"/>
+      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.33203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="16.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -606,7 +606,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -632,7 +632,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -658,7 +658,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
@@ -684,7 +684,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
@@ -707,7 +707,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
@@ -721,7 +721,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
@@ -735,7 +735,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
@@ -761,7 +761,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>42</v>
       </c>
@@ -790,7 +790,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>18</v>
       </c>
@@ -816,7 +816,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>23</v>
       </c>
@@ -842,7 +842,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>24</v>
       </c>
@@ -865,7 +865,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>26</v>
       </c>
@@ -891,7 +891,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>29</v>
       </c>
@@ -919,7 +919,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>30</v>
       </c>
@@ -945,7 +945,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>31</v>
       </c>
@@ -971,7 +971,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>32</v>
       </c>
@@ -994,7 +994,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>34</v>
       </c>
@@ -1008,7 +1008,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>35</v>
       </c>
@@ -1028,7 +1028,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>37</v>
       </c>
@@ -1054,7 +1054,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>38</v>
       </c>
@@ -1077,7 +1077,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>39</v>
       </c>
@@ -1100,7 +1100,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>40</v>
       </c>
@@ -1120,7 +1120,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>45</v>
       </c>
@@ -1137,7 +1137,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>46</v>
       </c>
@@ -1160,7 +1160,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>48</v>
       </c>
@@ -1191,53 +1191,48 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17CF9D33-C227-4C81-AA1E-9768BF33F1E6}">
-  <dimension ref="B2:C7"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="8.88671875" style="1"/>
-    <col min="3" max="3" width="84.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="8.85546875" style="1"/>
+    <col min="2" max="2" width="84.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
       <c r="B2" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
       <c r="B4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B5" s="1">
-        <v>1</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B6" s="1">
-        <v>2</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B7" s="1">
-        <v>3</v>
-      </c>
-      <c r="C7" s="1" t="s">
         <v>47</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add antenna gain function and update radar list.
</commit_message>
<xml_diff>
--- a/radars.xlsx
+++ b/radars.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tj\Documents\Engineering\Radar Cross Section\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCD57370-8CBC-4FFA-9B3E-049DA1CADADA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F5CC8A8-6BB8-4DDF-850D-93F39EF1A3C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15870" yWindow="9840" windowWidth="27060" windowHeight="15600" xr2:uid="{4644795B-AF5F-4458-9974-60729102D395}"/>
+    <workbookView xWindow="8745" yWindow="7995" windowWidth="19695" windowHeight="21285" xr2:uid="{4644795B-AF5F-4458-9974-60729102D395}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="58">
   <si>
     <t>Name</t>
   </si>
@@ -200,6 +200,15 @@
   </si>
   <si>
     <t>Thoth</t>
+  </si>
+  <si>
+    <t>MOTR</t>
+  </si>
+  <si>
+    <t>ISRO</t>
+  </si>
+  <si>
+    <t>http://www.indino.in/motr-indigenously-built-multi-object-tracking-radar-by-isro/</t>
   </si>
 </sst>
 </file>
@@ -557,11 +566,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CC53F9D-F6CF-438A-98EE-1DE843C93E8B}">
-  <dimension ref="A1:I26"/>
+  <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
+      <selection pane="bottomLeft" activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -570,7 +579,7 @@
     <col min="2" max="2" width="16.5703125" style="1" customWidth="1"/>
     <col min="3" max="3" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.28515625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
@@ -1183,6 +1192,29 @@
         <v>3</v>
       </c>
     </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C27" s="1">
+        <v>1.35</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E27" s="1">
+        <v>830</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I27" s="1">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1191,10 +1223,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17CF9D33-C227-4C81-AA1E-9768BF33F1E6}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1236,6 +1268,14 @@
         <v>47</v>
       </c>
     </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>